<commit_message>
Update: Se Modifica Aplicativo
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/02- Punto_Critico/01- Punto_Critico.xlsx
+++ b/6- VI_Trimestre/02- Punto_Critico/01- Punto_Critico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\02- Punto_Critico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296488F2-C327-475B-917E-82DA88FB5115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA635E8B-2953-47D2-B5BF-255AADA19335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="149">
   <si>
     <t>Puntos Criticos</t>
   </si>
@@ -131,6 +131,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>/</t>
     </r>
@@ -139,6 +140,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Andres Olaya</t>
     </r>
@@ -147,6 +149,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>/</t>
     </r>
@@ -155,6 +158,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Angela Rozo.</t>
     </r>
@@ -316,6 +320,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -324,6 +329,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Hardware - Software</t>
     </r>
@@ -333,6 +339,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>)</t>
     </r>
@@ -532,6 +539,9 @@
   <si>
     <t>Agregando la información faltante</t>
   </si>
+  <si>
+    <t>ISO 27002</t>
+  </si>
 </sst>
 </file>
 
@@ -551,60 +561,71 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1304,7 +1325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1436,9 +1457,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1452,6 +1470,28 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1475,28 +1515,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1753,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1836,12 +1854,12 @@
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1872,9 +1890,9 @@
       <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="83"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="94"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1905,9 +1923,9 @@
       <c r="D5" s="8">
         <v>1803170</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="94"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1931,16 +1949,16 @@
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="88"/>
+      <c r="C6" s="99"/>
       <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="94"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1971,9 +1989,9 @@
       <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="83"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="94"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2004,9 +2022,9 @@
       <c r="D8" s="9">
         <v>43500</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="83"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="94"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2030,16 +2048,16 @@
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="88"/>
+      <c r="C9" s="99"/>
       <c r="D9" s="9">
         <v>44000</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="83"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="94"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2070,9 +2088,9 @@
       <c r="D10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="86"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="97"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2100,12 +2118,12 @@
         <v>11</v>
       </c>
       <c r="C11" s="7"/>
-      <c r="D11" s="89" t="s">
+      <c r="D11" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="91"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="80"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2133,12 +2151,12 @@
         <v>13</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="92" t="s">
+      <c r="D12" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="91"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="80"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2162,16 +2180,16 @@
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="94"/>
-      <c r="D13" s="95" t="s">
+      <c r="C13" s="82"/>
+      <c r="D13" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="97"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2444,7 +2462,7 @@
       <c r="K19" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="101" t="s">
+      <c r="L19" s="77" t="s">
         <v>43</v>
       </c>
       <c r="M19" s="1"/>
@@ -2483,10 +2501,10 @@
       <c r="G20" s="39">
         <v>5</v>
       </c>
-      <c r="H20" s="99" t="s">
+      <c r="H20" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="I20" s="99" t="s">
+      <c r="I20" s="75" t="s">
         <v>142</v>
       </c>
       <c r="J20" s="34" t="s">
@@ -2495,7 +2513,7 @@
       <c r="K20" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="100" t="s">
+      <c r="L20" s="76" t="s">
         <v>34</v>
       </c>
       <c r="M20" s="1"/>
@@ -2585,7 +2603,7 @@
       <c r="G22" s="39">
         <v>5</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="74" t="s">
         <v>52</v>
       </c>
       <c r="I22" s="40" t="s">
@@ -2928,10 +2946,10 @@
       <c r="G29" s="39">
         <v>5</v>
       </c>
-      <c r="H29" s="99" t="s">
+      <c r="H29" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="I29" s="99" t="s">
+      <c r="I29" s="75" t="s">
         <v>144</v>
       </c>
       <c r="J29" s="34" t="s">
@@ -2979,10 +2997,10 @@
       <c r="G30" s="39">
         <v>9</v>
       </c>
-      <c r="H30" s="99" t="s">
+      <c r="H30" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="I30" s="99" t="s">
+      <c r="I30" s="75" t="s">
         <v>144</v>
       </c>
       <c r="J30" s="34" t="s">
@@ -3549,10 +3567,10 @@
       <c r="G42" s="32">
         <v>9</v>
       </c>
-      <c r="H42" s="99" t="s">
+      <c r="H42" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="I42" s="99" t="s">
+      <c r="I42" s="75" t="s">
         <v>147</v>
       </c>
       <c r="J42" s="34" t="s">
@@ -4373,8 +4391,10 @@
       <c r="B59" s="56">
         <v>37</v>
       </c>
-      <c r="C59" s="69"/>
-      <c r="D59" s="70" t="s">
+      <c r="C59" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="69" t="s">
         <v>135</v>
       </c>
       <c r="E59" s="44">
@@ -4456,7 +4476,7 @@
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="71">
+      <c r="B61" s="70">
         <v>38</v>
       </c>
       <c r="C61" s="22" t="s">
@@ -4465,10 +4485,10 @@
       <c r="D61" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="E61" s="72">
+      <c r="E61" s="71">
         <v>43941</v>
       </c>
-      <c r="F61" s="72">
+      <c r="F61" s="71">
         <v>43945</v>
       </c>
       <c r="G61" s="33">
@@ -4507,11 +4527,13 @@
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="73">
+      <c r="B62" s="72">
         <v>39</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="74" t="s">
+      <c r="C62" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="73" t="s">
         <v>0</v>
       </c>
       <c r="E62" s="32"/>
@@ -4540,11 +4562,13 @@
     </row>
     <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="73">
+      <c r="B63" s="72">
         <v>40</v>
       </c>
       <c r="C63" s="22"/>
-      <c r="D63" s="52"/>
+      <c r="D63" s="52" t="s">
+        <v>148</v>
+      </c>
       <c r="E63" s="32"/>
       <c r="F63" s="32"/>
       <c r="G63" s="32"/>
@@ -4571,7 +4595,7 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="73">
+      <c r="B64" s="72">
         <v>41</v>
       </c>
       <c r="C64" s="22"/>

</xml_diff>